<commit_message>
Cosas de la zona Tomb
</commit_message>
<xml_diff>
--- a/src/docs/chances.xlsx
+++ b/src/docs/chances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Datos\Personal\Godot\proyectos\quantum-platformer\src\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3123F35F-4571-4B30-9294-EEB610D7D6EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7203820-F3B4-4086-BC50-2823BB051C60}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B8D3B8E1-4551-41BC-8A8B-660CE6CF96C2}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
   <si>
     <t>Leaf</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Tumbas (Fantasma)</t>
+  </si>
+  <si>
+    <t>Cadenas Colgantes</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,7 +667,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
@@ -679,7 +682,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="16"/>
       <c r="B4" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
@@ -694,7 +697,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -708,8 +711,8 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="17"/>
-      <c r="B6" s="14" t="s">
-        <v>7</v>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -811,7 +814,9 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="12"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
         <v>22</v>
@@ -861,10 +866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A778086-87B7-4BBF-8A9B-F7080743C94B}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -990,6 +995,11 @@
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>